<commit_message>
GGWP T:N/A S0 - Actualización de US al nuevo formato
Solo se pasaron las 40 US de la primer hoja del documento al nuevo formato en la segunda hoja. Se fijó la primer fila del documento para mantener el titulo de las columnas.

Co-Authored-By: Ismael David Funes <ismafunes@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/proyecto/documentos/Descripción user stories.xlsx
+++ b/proyecto/documentos/Descripción user stories.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsmaFunes\Documents\Repositories\GitHub\GGWP\proyecto\documentos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
   </bookViews>
@@ -15,12 +10,12 @@
     <sheet name="Descripción de US" sheetId="1" r:id="rId1"/>
     <sheet name="Nueva descripción" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="180">
   <si>
     <t>USN</t>
   </si>
@@ -103,9 +98,6 @@
     <t>Consultar Usuario</t>
   </si>
   <si>
-    <t>Yo, como administrador quiero consultar los usuarios para poder conocer los usuarios actuales y sus permisos.</t>
-  </si>
-  <si>
     <t>Modificar Usuario</t>
   </si>
   <si>
@@ -298,9 +290,6 @@
     <t>Quiero &lt;acción&gt;</t>
   </si>
   <si>
-    <t>Para poder &lt;meta&gt;</t>
-  </si>
-  <si>
     <t>Recepcionista</t>
   </si>
   <si>
@@ -448,9 +437,6 @@
     <t>Ver los datos actualizados de éste.</t>
   </si>
   <si>
-    <t>Actualizar su información</t>
-  </si>
-  <si>
     <t>Tener información sobre los socios activos del gimnasio.</t>
   </si>
   <si>
@@ -464,6 +450,111 @@
   </si>
   <si>
     <t>Tener registro de los pagos de los socios, así como la fecha en la que pagaron</t>
+  </si>
+  <si>
+    <t>Actualizar su información.</t>
+  </si>
+  <si>
+    <t>Tener información sobre los pagos.</t>
+  </si>
+  <si>
+    <t>Cancelar un pago no efectuado o no deseado.</t>
+  </si>
+  <si>
+    <t>Conocer un usuario actual y sus permisos.</t>
+  </si>
+  <si>
+    <t>Yo, como administrador quiero consultar un usuario para conocer sus permisos.</t>
+  </si>
+  <si>
+    <t>Agregarle o modificar datos.</t>
+  </si>
+  <si>
+    <t>Que ya no tenga acceso al sistema.</t>
+  </si>
+  <si>
+    <t>Llevar un segumiento y control de la asistencia de un socio.</t>
+  </si>
+  <si>
+    <t>Tener registro de la cantidad de tiempo que el socio estuvo en el gimnasio.</t>
+  </si>
+  <si>
+    <t>Obtener información que me permita llevar un control de la cantidad de socios que se encuentran actualmente en el establecimiento.</t>
+  </si>
+  <si>
+    <t>Obtener información específica sobre la asistencia del socio en cierto período.</t>
+  </si>
+  <si>
+    <t>Imprimir y entregarle al cliente como comprobante.</t>
+  </si>
+  <si>
+    <t>Tener registradas las actividades y vincularlas a un plan.</t>
+  </si>
+  <si>
+    <t>Conocer sus datos.</t>
+  </si>
+  <si>
+    <t>Modificar los datos de una actividad.</t>
+  </si>
+  <si>
+    <t>Asignarlo a una rutina.</t>
+  </si>
+  <si>
+    <t>Ver sus datos.</t>
+  </si>
+  <si>
+    <t>Actualizar sus datos.</t>
+  </si>
+  <si>
+    <t>Asignarla a un socio.</t>
+  </si>
+  <si>
+    <t>Conocer sus ejercicios por día.</t>
+  </si>
+  <si>
+    <t>Actualizar sus ejercicios y sus días.</t>
+  </si>
+  <si>
+    <t>Para poder/que &lt;meta&gt;</t>
+  </si>
+  <si>
+    <t>Ya no esté mas en el sistema.</t>
+  </si>
+  <si>
+    <t>Ya no esté más en el sistema.</t>
+  </si>
+  <si>
+    <t>No exista más en el sistema.</t>
+  </si>
+  <si>
+    <t>Los empleados puedan tener usuarios con permisos a determinadas cosas.</t>
+  </si>
+  <si>
+    <t>Tenerla en papel.</t>
+  </si>
+  <si>
+    <t>Asignarselo a un socio.</t>
+  </si>
+  <si>
+    <t>Obtener información sobre éste.</t>
+  </si>
+  <si>
+    <t>Asignarsela a un ejercicio que la utilice.</t>
+  </si>
+  <si>
+    <t>Ver los datos de una máquina.</t>
+  </si>
+  <si>
+    <t>Ya no esté disponible para su utilización.</t>
+  </si>
+  <si>
+    <t>Tener acceso al sistema.</t>
+  </si>
+  <si>
+    <t>Salir del sistema.</t>
+  </si>
+  <si>
+    <t>Ya no exista más en el sistema.</t>
   </si>
 </sst>
 </file>
@@ -701,23 +792,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7030A0"/>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7030A0"/>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -806,7 +881,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -841,7 +916,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1018,7 +1093,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1031,15 +1106,15 @@
   </sheetPr>
   <dimension ref="A1:N212"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="47" customWidth="1"/>
+    <col min="3" max="3" width="55.140625" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" customWidth="1"/>
   </cols>
@@ -1052,7 +1127,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D1" s="24" t="s">
         <v>2</v>
@@ -1305,7 +1380,7 @@
         <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>27</v>
+        <v>149</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>25</v>
@@ -1325,10 +1400,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>25</v>
@@ -1348,10 +1423,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>25</v>
@@ -1371,13 +1446,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="E15" s="5"/>
       <c r="H15" s="5"/>
@@ -1394,13 +1469,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" s="5"/>
       <c r="H16" s="5"/>
@@ -1417,13 +1492,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" s="5"/>
       <c r="H17" s="5"/>
@@ -1440,13 +1515,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" s="5"/>
       <c r="H18" s="5"/>
@@ -1463,10 +1538,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>18</v>
@@ -1486,13 +1561,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="E20" s="5"/>
       <c r="H20" s="5"/>
@@ -1509,13 +1584,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="D21" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E21" s="5"/>
       <c r="H21" s="5"/>
@@ -1532,13 +1607,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="D22" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E22" s="5"/>
       <c r="H22" s="5"/>
@@ -1555,13 +1630,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="D23" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E23" s="5"/>
       <c r="H23" s="5"/>
@@ -1578,13 +1653,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="E24" s="5"/>
       <c r="H24" s="5"/>
@@ -1601,13 +1676,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D25" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E25" s="5"/>
       <c r="H25" s="5"/>
@@ -1624,13 +1699,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="D26" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E26" s="5"/>
       <c r="H26" s="5"/>
@@ -1647,13 +1722,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="D27" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E27" s="5"/>
       <c r="H27" s="5"/>
@@ -1670,13 +1745,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="E28" s="5"/>
       <c r="H28" s="5"/>
@@ -1693,13 +1768,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="D29" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E29" s="5"/>
       <c r="H29" s="5"/>
@@ -1716,13 +1791,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="D30" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E30" s="5"/>
       <c r="H30" s="5"/>
@@ -1739,13 +1814,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="D31" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E31" s="5"/>
       <c r="H31" s="5"/>
@@ -1762,13 +1837,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>81</v>
-      </c>
       <c r="D32" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E32" s="5"/>
       <c r="H32" s="5"/>
@@ -1785,13 +1860,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="E33" s="5"/>
       <c r="H33" s="5"/>
@@ -1808,13 +1883,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E34" s="5"/>
       <c r="H34" s="5"/>
@@ -1831,13 +1906,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="D35" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E35" s="5"/>
       <c r="H35" s="5"/>
@@ -1854,13 +1929,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="D36" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E36" s="5"/>
       <c r="H36" s="5"/>
@@ -1877,13 +1952,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="D37" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E37" s="5"/>
       <c r="H37" s="5"/>
@@ -1900,13 +1975,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="D38" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E38" s="5"/>
       <c r="H38" s="5"/>
@@ -1923,13 +1998,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>78</v>
-      </c>
       <c r="D39" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E39" s="5"/>
       <c r="H39" s="5"/>
@@ -1946,10 +2021,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D40" s="21" t="s">
         <v>25</v>
@@ -1969,10 +2044,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D41" s="10" t="s">
         <v>25</v>
@@ -3620,7 +3695,8 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3629,10 +3705,10 @@
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3640,19 +3716,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>91</v>
-      </c>
       <c r="E1" s="20" t="s">
-        <v>92</v>
+        <v>166</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <f>1</f>
         <v>1</v>
@@ -3661,19 +3737,19 @@
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <f t="shared" ref="A3:A41" si="0">A2+1</f>
         <v>2</v>
@@ -3682,13 +3758,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>5</v>
@@ -3703,19 +3779,19 @@
         <v>8</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3724,19 +3800,19 @@
         <v>10</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3745,19 +3821,19 @@
         <v>12</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3766,19 +3842,19 @@
         <v>14</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3787,13 +3863,13 @@
         <v>16</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>18</v>
@@ -3808,17 +3884,19 @@
         <v>19</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E9" s="5"/>
+        <v>104</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>146</v>
+      </c>
       <c r="F9" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3827,17 +3905,19 @@
         <v>21</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E10" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>147</v>
+      </c>
       <c r="F10" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3846,17 +3926,19 @@
         <v>23</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E11" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>170</v>
+      </c>
       <c r="F11" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3865,31 +3947,35 @@
         <v>26</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="E12" s="5"/>
+        <v>107</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>148</v>
+      </c>
       <c r="F12" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E13" s="5"/>
+        <v>108</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>150</v>
+      </c>
       <c r="F13" s="3" t="s">
         <v>25</v>
       </c>
@@ -3900,110 +3986,122 @@
         <v>13</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E14" s="5"/>
+        <v>109</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>151</v>
+      </c>
       <c r="F14" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="5" t="s">
+      <c r="C16" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D16" s="5" t="s">
+      <c r="E17" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="E18" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="E19" s="5"/>
+      <c r="E19" s="5" t="s">
+        <v>156</v>
+      </c>
       <c r="F19" s="3" t="s">
         <v>18</v>
       </c>
@@ -4014,55 +4112,61 @@
         <v>19</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="E22" s="5"/>
+      <c r="E22" s="5" t="s">
+        <v>159</v>
+      </c>
       <c r="F22" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.2">
@@ -4071,17 +4175,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E23" s="5"/>
+        <v>119</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>167</v>
+      </c>
       <c r="F23" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.2">
@@ -4090,17 +4196,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="E24" s="5"/>
+        <v>120</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>160</v>
+      </c>
       <c r="F24" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.2">
@@ -4109,17 +4217,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="E25" s="5"/>
+        <v>121</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>161</v>
+      </c>
       <c r="F25" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.2">
@@ -4128,17 +4238,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="E26" s="5"/>
+        <v>122</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="F26" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.2">
@@ -4147,17 +4259,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="E27" s="5"/>
+        <v>123</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>168</v>
+      </c>
       <c r="F27" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.2">
@@ -4166,17 +4280,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="E28" s="5"/>
+        <v>124</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>163</v>
+      </c>
       <c r="F28" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.2">
@@ -4185,17 +4301,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="E29" s="5"/>
+        <v>125</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>164</v>
+      </c>
       <c r="F29" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.2">
@@ -4204,17 +4322,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E30" s="5"/>
+        <v>126</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>165</v>
+      </c>
       <c r="F30" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.2">
@@ -4223,17 +4343,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="E31" s="5"/>
+        <v>127</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>179</v>
+      </c>
       <c r="F31" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.2">
@@ -4242,17 +4364,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="E32" s="5"/>
+        <v>128</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="F32" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.2">
@@ -4261,17 +4385,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="E33" s="5"/>
+        <v>129</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>172</v>
+      </c>
       <c r="F33" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.2">
@@ -4280,17 +4406,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="E34" s="5"/>
+        <v>130</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>173</v>
+      </c>
       <c r="F34" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.2">
@@ -4299,17 +4427,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="E35" s="5"/>
+        <v>131</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="F35" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.2">
@@ -4318,17 +4448,19 @@
         <v>35</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="E36" s="5"/>
+        <v>132</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>169</v>
+      </c>
       <c r="F36" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.2">
@@ -4337,17 +4469,19 @@
         <v>36</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="E37" s="5"/>
+        <v>133</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>174</v>
+      </c>
       <c r="F37" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.2">
@@ -4356,17 +4490,19 @@
         <v>37</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="E38" s="5"/>
+        <v>134</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>175</v>
+      </c>
       <c r="F38" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.2">
@@ -4375,53 +4511,59 @@
         <v>38</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="E39" s="5"/>
+        <v>135</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>176</v>
+      </c>
       <c r="F39" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="E40" s="5"/>
+        <v>136</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>177</v>
+      </c>
       <c r="F40" s="21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E41" s="5"/>
+        <v>137</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>178</v>
+      </c>
       <c r="F41" s="21" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
GGWP T:N/A S0 - Descripción de user stories
Se agrega Registrar Socio, Modificar Socio y Consultar Socio
</commit_message>
<xml_diff>
--- a/proyecto/documentos/Descripción user stories.xlsx
+++ b/proyecto/documentos/Descripción user stories.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsmaFunes\Documents\Repositories\GitHub\GGWP\proyecto\documentos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
   </bookViews>
@@ -10,7 +15,7 @@
     <sheet name="Descripción de US" sheetId="1" r:id="rId1"/>
     <sheet name="Nueva descripción" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -452,9 +457,6 @@
     <t>Tener registro de los pagos de los socios, así como la fecha en la que pagaron</t>
   </si>
   <si>
-    <t>Actualizar su información.</t>
-  </si>
-  <si>
     <t>Tener información sobre los pagos.</t>
   </si>
   <si>
@@ -555,6 +557,9 @@
   </si>
   <si>
     <t>Ya no exista más en el sistema.</t>
+  </si>
+  <si>
+    <t>Actualizar sus datos y tenerlos siempre al día.</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1098,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1380,7 +1385,7 @@
         <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>25</v>
@@ -1992,7 +1997,7 @@
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
     </row>
-    <row r="39" spans="1:14" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -3695,8 +3700,8 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3706,6 +3711,7 @@
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
     <col min="5" max="5" width="44.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
@@ -3722,7 +3728,7 @@
         <v>90</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -3770,7 +3776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3785,7 +3791,7 @@
         <v>100</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>145</v>
+        <v>179</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>5</v>
@@ -3854,7 +3860,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3890,7 +3896,7 @@
         <v>104</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>18</v>
@@ -3911,7 +3917,7 @@
         <v>105</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>18</v>
@@ -3932,7 +3938,7 @@
         <v>106</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>25</v>
@@ -3953,7 +3959,7 @@
         <v>107</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>25</v>
@@ -3974,7 +3980,7 @@
         <v>108</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>25</v>
@@ -3995,7 +4001,7 @@
         <v>109</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>25</v>
@@ -4016,7 +4022,7 @@
         <v>110</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>32</v>
@@ -4037,13 +4043,13 @@
         <v>111</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -4058,7 +4064,7 @@
         <v>112</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>32</v>
@@ -4079,7 +4085,7 @@
         <v>113</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>32</v>
@@ -4100,7 +4106,7 @@
         <v>114</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>18</v>
@@ -4121,7 +4127,7 @@
         <v>116</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>39</v>
@@ -4142,7 +4148,7 @@
         <v>117</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>39</v>
@@ -4163,7 +4169,7 @@
         <v>118</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>39</v>
@@ -4184,7 +4190,7 @@
         <v>119</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>39</v>
@@ -4205,7 +4211,7 @@
         <v>120</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>48</v>
@@ -4226,7 +4232,7 @@
         <v>121</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>48</v>
@@ -4247,7 +4253,7 @@
         <v>122</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>48</v>
@@ -4268,7 +4274,7 @@
         <v>123</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>48</v>
@@ -4289,7 +4295,7 @@
         <v>124</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>57</v>
@@ -4310,7 +4316,7 @@
         <v>125</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>57</v>
@@ -4331,7 +4337,7 @@
         <v>126</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>57</v>
@@ -4352,7 +4358,7 @@
         <v>127</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>57</v>
@@ -4373,7 +4379,7 @@
         <v>128</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>57</v>
@@ -4394,7 +4400,7 @@
         <v>129</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>66</v>
@@ -4415,7 +4421,7 @@
         <v>130</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>66</v>
@@ -4436,7 +4442,7 @@
         <v>131</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>66</v>
@@ -4457,7 +4463,7 @@
         <v>132</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>66</v>
@@ -4478,7 +4484,7 @@
         <v>133</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>57</v>
@@ -4499,7 +4505,7 @@
         <v>134</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>57</v>
@@ -4520,7 +4526,7 @@
         <v>135</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F39" s="10" t="s">
         <v>57</v>
@@ -4541,7 +4547,7 @@
         <v>136</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F40" s="21" t="s">
         <v>25</v>
@@ -4562,7 +4568,7 @@
         <v>137</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F41" s="21" t="s">
         <v>25</v>

</xml_diff>